<commit_message>
Ajout des schémas elec V1 et des datasheets correspondantes
</commit_message>
<xml_diff>
--- a/Schémas Electriques/Mapping Pic.xlsx
+++ b/Schémas Electriques/Mapping Pic.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Mapping Carte V1.0" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="101">
   <si>
     <t>RA0</t>
   </si>
@@ -273,6 +273,51 @@
   </si>
   <si>
     <t>MCLR</t>
+  </si>
+  <si>
+    <t>CLOCK</t>
+  </si>
+  <si>
+    <t>I moteur</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>LED3</t>
+  </si>
+  <si>
+    <t>LED4</t>
+  </si>
+  <si>
+    <t>LED5</t>
+  </si>
+  <si>
+    <t>LED6</t>
+  </si>
+  <si>
+    <t>PWM moteur</t>
+  </si>
+  <si>
+    <t>Sens Moteur</t>
+  </si>
+  <si>
+    <t>SDL</t>
+  </si>
+  <si>
+    <t>Capteur1</t>
+  </si>
+  <si>
+    <t>Capteur2</t>
+  </si>
+  <si>
+    <t>Capteur3</t>
+  </si>
+  <si>
+    <t>Capteur4</t>
   </si>
 </sst>
 </file>
@@ -288,7 +333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,8 +406,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -671,11 +728,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -698,9 +766,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -714,6 +779,123 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -747,139 +929,31 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1191,19 +1265,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="11"/>
+    <col min="1" max="1" width="11.42578125" style="10"/>
     <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
     <col min="3" max="6" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="30" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1215,485 +1289,545 @@
       <c r="D1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="12"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51" t="s">
+      <c r="B2" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="37" t="s">
+      <c r="A3" s="52"/>
+      <c r="B3" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="54"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="37" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="31" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="63" t="s">
+      <c r="A5" s="52"/>
+      <c r="B5" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="32" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="63" t="s">
+      <c r="A6" s="52"/>
+      <c r="B6" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="32" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="37" t="s">
+      <c r="A7" s="52"/>
+      <c r="B7" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="54"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="37" t="s">
+      <c r="A8" s="52"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="54" t="s">
+      <c r="F8" s="31" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="38" t="s">
+      <c r="A9" s="53"/>
+      <c r="B9" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="38" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="39" t="s">
+      <c r="B10" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="62"/>
+      <c r="F10" s="39"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="40" t="s">
+      <c r="A11" s="55"/>
+      <c r="B11" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="54"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="40" t="s">
+      <c r="A12" s="55"/>
+      <c r="B12" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="54"/>
+      <c r="F12" s="31"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="40" t="s">
+      <c r="A13" s="55"/>
+      <c r="B13" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="54"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="40" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="54"/>
+      <c r="F14" s="31"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="40" t="s">
+      <c r="A15" s="55"/>
+      <c r="B15" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="54"/>
+      <c r="F15" s="31"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="64" t="s">
+      <c r="A16" s="55"/>
+      <c r="B16" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="57" t="s">
+      <c r="E16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="54"/>
+      <c r="F16" s="31"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="65" t="s">
+      <c r="A17" s="56"/>
+      <c r="B17" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="61"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="42" t="s">
+      <c r="B18" s="45"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="62"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="39"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="43" t="s">
+      <c r="A19" s="58"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="54"/>
+      <c r="F19" s="31"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="43" t="s">
+      <c r="A20" s="58"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="54"/>
+      <c r="F20" s="31"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="43" t="s">
+      <c r="A21" s="58"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="54"/>
+      <c r="F21" s="31"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="43" t="s">
+      <c r="A22" s="58"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="54" t="s">
+      <c r="F22" s="31" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="43" t="s">
+      <c r="A23" s="58"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="54" t="s">
+      <c r="F23" s="31" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+      <c r="A24" s="58"/>
       <c r="B24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="57" t="s">
+      <c r="E24" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="54"/>
+      <c r="F24" s="31"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="58" t="s">
+      <c r="E25" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="61"/>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="69"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="45" t="s">
+      <c r="B26" s="45"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="62"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="46" t="s">
+      <c r="A27" s="61"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="54"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="31"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="46" t="s">
+      <c r="A28" s="61"/>
+      <c r="B28" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="54"/>
+      <c r="F28" s="31"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="46" t="s">
+      <c r="A29" s="61"/>
+      <c r="B29" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F29" s="54"/>
+      <c r="F29" s="31"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="46" t="s">
+      <c r="A30" s="61"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="54"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="31"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="46" t="s">
+      <c r="A31" s="61"/>
+      <c r="B31" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="F31" s="54"/>
+      <c r="F31" s="31"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="46" t="s">
+      <c r="A32" s="61"/>
+      <c r="B32" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F32" s="54"/>
+      <c r="F32" s="31"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="47" t="s">
+      <c r="A33" s="62"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="56" t="s">
+      <c r="E33" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="61"/>
+      <c r="F33" s="38"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="66"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="48" t="s">
+      <c r="B34" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="59" t="s">
+      <c r="E34" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="37"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="32"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="54"/>
+      <c r="F35" s="31"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
-      <c r="B36" s="67"/>
-      <c r="C36" s="32"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="54"/>
+      <c r="F36" s="31"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
-      <c r="B37" s="65" t="s">
+      <c r="A37" s="48"/>
+      <c r="B37" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="69" t="s">
         <v>26</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="58" t="s">
+      <c r="E37" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="61"/>
+      <c r="F37" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Ajout des schémas elec de wrapping V2 ainsi que d'une BOM
</commit_message>
<xml_diff>
--- a/Schémas Electriques/Mapping Pic.xlsx
+++ b/Schémas Electriques/Mapping Pic.xlsx
@@ -275,9 +275,6 @@
     <t>MCLR</t>
   </si>
   <si>
-    <t>CLOCK</t>
-  </si>
-  <si>
     <t>I moteur</t>
   </si>
   <si>
@@ -308,16 +305,19 @@
     <t>SDL</t>
   </si>
   <si>
-    <t>Capteur1</t>
-  </si>
-  <si>
-    <t>Capteur2</t>
-  </si>
-  <si>
-    <t>Capteur3</t>
-  </si>
-  <si>
-    <t>Capteur4</t>
+    <t>Capteur 1</t>
+  </si>
+  <si>
+    <t>Enable Capteur</t>
+  </si>
+  <si>
+    <t>Quartz2</t>
+  </si>
+  <si>
+    <t>Quartz1</t>
+  </si>
+  <si>
+    <t>Break</t>
   </si>
 </sst>
 </file>
@@ -878,6 +878,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -929,31 +953,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,20 +1289,18 @@
       <c r="D1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="50"/>
+      <c r="F1" s="58"/>
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="67" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="49" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="29" t="s">
@@ -1314,11 +1312,9 @@
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="68" t="s">
+      <c r="A3" s="60"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="17" t="s">
@@ -1330,11 +1326,9 @@
       <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="68" t="s">
+      <c r="A4" s="60"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="17" t="s">
@@ -1348,11 +1342,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="17" t="s">
@@ -1366,11 +1360,11 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="17" t="s">
@@ -1384,11 +1378,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="68" t="s">
+      <c r="A7" s="60"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="17" t="s">
@@ -1398,8 +1390,10 @@
       <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="43"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="40" t="s">
+        <v>98</v>
+      </c>
       <c r="C8" s="14"/>
       <c r="D8" s="17" t="s">
         <v>40</v>
@@ -1412,11 +1406,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
-      <c r="B9" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="69" t="s">
+      <c r="A9" s="61"/>
+      <c r="B9" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="51" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -1430,13 +1424,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="62" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="19" t="s">
@@ -1448,11 +1442,11 @@
       <c r="F10" s="39"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="66" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="48" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="20" t="s">
@@ -1464,11 +1458,11 @@
       <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="66" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="48" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="20" t="s">
@@ -1480,11 +1474,11 @@
       <c r="F12" s="31"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="48" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="20" t="s">
@@ -1496,11 +1490,11 @@
       <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="48" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="20" t="s">
@@ -1512,11 +1506,11 @@
       <c r="F14" s="31"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="48" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="20" t="s">
@@ -1528,11 +1522,11 @@
       <c r="F15" s="31"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
+      <c r="A16" s="63"/>
       <c r="B16" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="50" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="20" t="s">
@@ -1544,11 +1538,11 @@
       <c r="F16" s="31"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="56"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="51" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="21" t="s">
@@ -1560,7 +1554,7 @@
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="65" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="45"/>
@@ -1572,7 +1566,7 @@
       <c r="F18" s="39"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
+      <c r="A19" s="66"/>
       <c r="B19" s="43"/>
       <c r="C19" s="14"/>
       <c r="D19" s="23" t="s">
@@ -1584,8 +1578,10 @@
       <c r="F19" s="31"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
-      <c r="B20" s="43"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="23" t="s">
+        <v>97</v>
+      </c>
       <c r="C20" s="14"/>
       <c r="D20" s="23" t="s">
         <v>16</v>
@@ -1596,8 +1592,10 @@
       <c r="F20" s="31"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
-      <c r="B21" s="43"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="23" t="s">
+        <v>96</v>
+      </c>
       <c r="C21" s="14"/>
       <c r="D21" s="23" t="s">
         <v>17</v>
@@ -1608,7 +1606,7 @@
       <c r="F21" s="31"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="58"/>
+      <c r="A22" s="66"/>
       <c r="B22" s="43"/>
       <c r="C22" s="14"/>
       <c r="D22" s="23" t="s">
@@ -1622,9 +1620,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="58"/>
+      <c r="A23" s="66"/>
       <c r="B23" s="43"/>
-      <c r="C23" s="71"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="23" t="s">
         <v>19</v>
       </c>
@@ -1636,11 +1634,11 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="58"/>
+      <c r="A24" s="66"/>
       <c r="B24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="66" t="s">
+      <c r="C24" s="48" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="23" t="s">
@@ -1652,11 +1650,11 @@
       <c r="F24" s="31"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="59"/>
+      <c r="A25" s="67"/>
       <c r="B25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="69" t="s">
+      <c r="C25" s="51" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="24" t="s">
@@ -1668,7 +1666,7 @@
       <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="60" t="s">
+      <c r="A26" s="68" t="s">
         <v>53</v>
       </c>
       <c r="B26" s="45"/>
@@ -1680,7 +1678,7 @@
       <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="61"/>
+      <c r="A27" s="69"/>
       <c r="B27" s="43"/>
       <c r="C27" s="14"/>
       <c r="D27" s="26" t="s">
@@ -1690,7 +1688,7 @@
       <c r="F27" s="31"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="61"/>
+      <c r="A28" s="69"/>
       <c r="B28" s="40" t="s">
         <v>24</v>
       </c>
@@ -1704,9 +1702,9 @@
       <c r="F28" s="31"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="A29" s="69"/>
       <c r="B29" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="26" t="s">
@@ -1718,8 +1716,10 @@
       <c r="F29" s="31"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="61"/>
-      <c r="B30" s="64"/>
+      <c r="A30" s="69"/>
+      <c r="B30" s="71" t="s">
+        <v>94</v>
+      </c>
       <c r="C30" s="14"/>
       <c r="D30" s="26" t="s">
         <v>45</v>
@@ -1728,11 +1728,11 @@
       <c r="F30" s="31"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="61"/>
+      <c r="A31" s="69"/>
       <c r="B31" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="48" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="26" t="s">
@@ -1744,11 +1744,11 @@
       <c r="F31" s="31"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="61"/>
+      <c r="A32" s="69"/>
       <c r="B32" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="48" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="26" t="s">
@@ -1760,7 +1760,7 @@
       <c r="F32" s="31"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="62"/>
+      <c r="A33" s="70"/>
       <c r="B33" s="44"/>
       <c r="C33" s="16"/>
       <c r="D33" s="27" t="s">
@@ -1772,13 +1772,13 @@
       <c r="F33" s="38"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="65" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="67" t="s">
+      <c r="B34" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="49" t="s">
         <v>26</v>
       </c>
       <c r="D34" s="28" t="s">
@@ -1790,7 +1790,7 @@
       <c r="F34" s="37"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
+      <c r="A35" s="55"/>
       <c r="B35" s="43"/>
       <c r="C35" s="15"/>
       <c r="D35" s="6" t="s">
@@ -1802,7 +1802,7 @@
       <c r="F35" s="31"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
+      <c r="A36" s="55"/>
       <c r="B36" s="43"/>
       <c r="C36" s="15"/>
       <c r="D36" s="6" t="s">
@@ -1814,11 +1814,11 @@
       <c r="F36" s="31"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="48"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="69" t="s">
+      <c r="C37" s="51" t="s">
         <v>26</v>
       </c>
       <c r="D37" s="7" t="s">

</xml_diff>